<commit_message>
adjusting book images and text on pages
</commit_message>
<xml_diff>
--- a/Project Documentation/Stories.xlsx
+++ b/Project Documentation/Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bunnygotfangs/Documents/baby-build-a-book/Project Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5B6A2C-4ECA-9643-A582-909660391C48}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1218147B-878D-8140-A4CA-050C5F7277DF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{DDAF371D-486C-8843-95AA-86B876C35D2D}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>Page 1</t>
   </si>
   <si>
-    <t>Page</t>
-  </si>
-  <si>
     <t>Page 3</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Walk with ___{Char_Name} in the Park</t>
   </si>
   <si>
-    <t>I would travel in my ___{Fav_Color} rocket.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Inside my rocket, I would have ___{Fav_Food} to eat while I peek out the window and look at the stars. </t>
   </si>
   <si>
@@ -94,32 +88,13 @@
   </si>
   <si>
     <t>It was a bright, sunny summer day when ___{Char_Name} went to visit the beach with their parents and  best friend,  ____{BFF}.</t>
-  </si>
-  <si>
-    <t>“ ____{BFF}, can you help me find a shell today?” 
-“Sure, ___{Char_Name}  ”, answered ____{BFF}. 
-“What does it look like?”</t>
   </si>
   <si>
     <t>Today ___{Char_Name}  was looking for a very special shell.
  This shell would allow them to hear the ocean, even when they returned back home to the big city! Can you guess what kind of shell this is?</t>
   </si>
   <si>
-    <t>I bet if we had a ___{Fav_Animal} they could help us find the shell.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“Hmmmm”, thought ___{Char_Name} while eating ___{Fav_Food|. 
-“It’s big, ___{fav_Color}, has spines on it, and takes two hands to carry!” 
-“Ohhhhh, you want to find a conch shell!” exclaimed ____{BFF}.  </t>
-  </si>
-  <si>
-    <t>___{Char_Name}  loved going to the beach and ___{Fav_Actvitiy} in the water and wave at the fish swimming by. Often they ould nme the fish after ___{Fav_Char}</t>
-  </si>
-  <si>
     <t>Once upon a time there was a little bear named ___{Char_Name}.</t>
-  </si>
-  <si>
-    <t>___{Char_Name} in lived in a little ___{Fav_Color} treehouse surronded by flowers and streams.</t>
   </si>
   <si>
     <t>___{Char_Name}'s best friend was another little bear named ___{BFF_Name}</t>
@@ -156,6 +131,27 @@
   </si>
   <si>
     <t>When we aren't at the zoo, or riding the carousel, we often play ___{Fav_Activity} or pretending to be ___{Fav_Char}.</t>
+  </si>
+  <si>
+    <t>___{Char_Name}  loved going to the beach and ___{Fav_Actvitiy} in the water and wave at the fish swimming by. Often they would name the fish after ___{Fav_Char}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is a special shell they were looking for. As it was big and bright and ___{fav_Color}. They looked for it in the water and they looked for it in the sand. </t>
+  </si>
+  <si>
+    <t>Page 2</t>
+  </si>
+  <si>
+    <t>___{Char_Name} lived in a little ___{Fav_Color} treehouse surronded by flowers and streams. They also lived with their favorite animal, ___{fav_Animal}</t>
+  </si>
+  <si>
+    <t>They looked everywhere for the special shell, but sadly they did not find it. While searching though they came across a food cart, that was selling ___{fav_food}, so they enjoyed a snack together.</t>
+  </si>
+  <si>
+    <t>I bet if we had a ___{Fav_Animal} they could help us find the shel</t>
+  </si>
+  <si>
+    <t>I would travel in my ___{Fav_Color} rocket. If I could I would bring ___{fav_animal} to keep me company.</t>
   </si>
 </sst>
 </file>
@@ -530,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9817000C-BA85-CE49-862A-BD8F271F8A20}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A19"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -549,7 +545,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -558,123 +554,123 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="162" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="162" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="126" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>